<commit_message>
practica excel, se quito ejercicios resueltos
</commit_message>
<xml_diff>
--- a/excel/Ventas_del_año.xlsx
+++ b/excel/Ventas_del_año.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git-practice\Git-practice\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Git-practice\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51909EB2-FE05-4CEB-BCC2-98D27AEE5414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AA51826-1E50-456E-B184-8B8EC3B39B92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{62DEE931-8AC8-4954-A7A9-883E10260878}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{62DEE931-8AC8-4954-A7A9-883E10260878}"/>
   </bookViews>
   <sheets>
     <sheet name="Ventas diarias" sheetId="7" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="82">
   <si>
     <t>Fecha</t>
   </si>
@@ -258,9 +258,6 @@
     <t>concatenado</t>
   </si>
   <si>
-    <t xml:space="preserve">  </t>
-  </si>
-  <si>
     <t>añadir fecha de hoy</t>
   </si>
   <si>
@@ -289,6 +286,12 @@
   </si>
   <si>
     <t>venta * utilida %</t>
+  </si>
+  <si>
+    <t>En la parte de arriba</t>
+  </si>
+  <si>
+    <t>quiero ver siempre ver los titulos</t>
   </si>
 </sst>
 </file>
@@ -797,7 +800,7 @@
   <dimension ref="A1:L152"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -863,7 +866,7 @@
         <v>44562</v>
       </c>
       <c r="L2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -926,9 +929,6 @@
       <c r="I4">
         <v>44564</v>
       </c>
-      <c r="L4" t="s">
-        <v>73</v>
-      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -987,6 +987,9 @@
       <c r="I6">
         <v>44566</v>
       </c>
+      <c r="L6" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -1016,6 +1019,9 @@
       <c r="I7">
         <v>44567</v>
       </c>
+      <c r="L7" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -1045,6 +1051,9 @@
       <c r="I8">
         <v>44568</v>
       </c>
+      <c r="L8" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -5224,6 +5233,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5231,7 +5241,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D472B34-EC61-4597-AA4B-208FB0ADC221}">
   <dimension ref="B2:K18"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
@@ -5307,7 +5317,7 @@
         <v>0.5420016760557832</v>
       </c>
       <c r="G4" s="18">
-        <f t="shared" ref="G4:G8" si="2">F4*C4</f>
+        <f t="shared" ref="G4:G7" si="2">F4*C4</f>
         <v>59993.320000000007</v>
       </c>
     </row>
@@ -5417,37 +5427,37 @@
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="F12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="F13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="F14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="F15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="F16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -5772,14 +5782,14 @@
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B9">
         <f ca="1">RAND()</f>
-        <v>0.69344115680526119</v>
+        <v>1.8782293890518664E-2</v>
       </c>
       <c r="C9" s="3"/>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B10">
         <f ca="1">RANDBETWEEN(1,5)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C10" s="3"/>
       <c r="E10" s="3"/>
@@ -5787,7 +5797,7 @@
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C11" s="3"/>
       <c r="E11" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
@@ -5798,13 +5808,13 @@
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.25">
       <c r="K14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H15" s="10"/>
       <c r="K15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -5818,8 +5828,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A8B5EE8-73A7-413E-B211-7350E9466C03}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5846,7 +5856,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="b">
-        <f t="shared" ref="B2:B9" si="0">A2=A3</f>
+        <f t="shared" ref="B2:B8" si="0">A2=A3</f>
         <v>0</v>
       </c>
       <c r="C2" t="b">
@@ -5861,9 +5871,6 @@
       <c r="B3" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>